<commit_message>
re-ordered columns and converted cols to numeric
</commit_message>
<xml_diff>
--- a/results/output_unified_duration_cms_test_archive_2025.07.09.xlsx
+++ b/results/output_unified_duration_cms_test_archive_2025.07.09.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinzhao/DS_Projects/semiauto-epi-data-extraction-pipeline/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3200EC63-4035-0D4E-8540-759AC7050794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDB2A56-CBC1-FA4A-8682-1ADAEE25E75A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="69">
   <si>
     <t>File</t>
   </si>
@@ -225,13 +225,16 @@
   </si>
   <si>
     <t xml:space="preserve">Apply parse_dates() </t>
+  </si>
+  <si>
+    <t>pd.to_numeric()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,6 +251,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
@@ -256,12 +266,17 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -303,21 +318,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -660,7 +677,7 @@
   <dimension ref="A1:AB15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -862,68 +879,71 @@
       </c>
     </row>
     <row r="7" spans="1:28" ht="19" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
+    <row r="8" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="B8" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
+    <row r="9" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="B9" s="4" t="s">
         <v>54</v>
       </c>
       <c r="C9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+    <row r="10" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="B10" s="4" t="s">
         <v>55</v>
       </c>
       <c r="C10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
+    <row r="11" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="B11" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
+    <row r="12" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="B12" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C12" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
+    <row r="13" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="B13" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C13" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
+    <row r="14" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="B14" s="4" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
+      <c r="C14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="B15" s="4" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>